<commit_message>
corrigir looping e deixar async
</commit_message>
<xml_diff>
--- a/dados_acumulados.xlsx
+++ b/dados_acumulados.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,431 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>abertura</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>situacao</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>tipo</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>porte</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>natureza_juridica</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>atividade_principal</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>qsa</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>logradouro</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>numero</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>municipio</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>bairro</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>uf</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>cep</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>telefone</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>data_situacao</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>cnpj</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>ultima_atualizacao</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>status</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>fantasia</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>complemento</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>efr</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>motivo_situacao</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>situacao_especial</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>data_situacao_especial</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>atividades_secundarias</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>capital_social</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>extra</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>billing</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>02/01/1969</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ATIVA</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>MATRIZ</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>COMERCIO DE BORRACHAS TATUAPE LTDA</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>EMPRESA DE PEQUENO PORTE</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>206-2 - Sociedade Empresária Limitada</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>[{'code': '47.89-0-99', 'text': 'Comércio varejista de outros produtos não especificados anteriormente'}]</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>[{'nome': 'WALDOMIRO DE OLIVEIRA MACHADO', 'qual': '49-Sócio-Administrador'}]</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>RUA DOUTOR JOSE DO AMARAL</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>235</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>SAO PAULO</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>JARDIM LISBOA</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>03.675-010</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>jaime.penteado@terra.com.br</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>(11) 3756-3380</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>04/06/2005</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>61.377.933/0001-97</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>2023-10-14T23:59:59.000Z</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>[{'code': '00.00-0-00', 'text': 'Não informada'}]</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>200000.00</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>{'free': True, 'database': True}</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>09/10/2017</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ATIVA</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MATRIZ</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>LUZ LED ILUMINACAO LTDA</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>MICRO EMPRESA</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>206-2 - Sociedade Empresária Limitada</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>[{'code': '46.93-1-00', 'text': 'Comércio atacadista de mercadorias em geral, sem predominância de alimentos ou de insumos agropecuários'}]</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>[{'nome': 'VALERIA LIMA DE SOUZA', 'qual': '49-Sócio-Administrador'}]</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>AVENIDA ATILIO BRUGNOLI</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>188</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>SAO PAULO</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>PARQUE NACOES UNIDAS</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>02.996-010</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>financeiro@luzatual.com.br</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>(11) 2385-1513 / (11) 2385-1514 / (11) 3978-7005</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>09/10/2017</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>28.819.515/0001-37</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>2023-11-11T23:59:59.000Z</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>LUZ LED</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>CASA 3</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>[{'code': '33.13-9-99', 'text': 'Manutenção e reparação de máquinas, aparelhos e materiais elétricos não especificados anteriormente'}, {'code': '33.29-5-99', 'text': 'Instalação de outros equipamentos não especificados anteriormente'}, {'code': '43.21-5-00', 'text': 'Instalações elétricas'}, {'code': '46.49-4-02', 'text': 'Comércio atacadista de aparelhos eletrônicos de uso pessoal e doméstico'}, {'code': '46.72-9-00', 'text': 'Comércio atacadista de ferragens e ferramentas'}, {'code': '47.42-3-00', 'text': 'Comércio varejista de material elétrico'}, {'code': '71.12-0-00', 'text': 'Serviços de engenharia'}]</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>95000.00</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>{'free': True, 'database': True}</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>